<commit_message>
🗃️ (TST_Srinivasan_2021-10_FA): fix date
FIX #58
</commit_message>
<xml_diff>
--- a/Data/raw/TST_Srinivasan_2021-10_FA/TST_2021-10_FA_metadata.xlsx
+++ b/Data/raw/TST_Srinivasan_2021-10_FA/TST_2021-10_FA_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="1" state="visible" r:id="rId2"/>
@@ -143,7 +143,7 @@
     <t xml:space="preserve">Dharun Vadugappatty Srinivasan</t>
   </si>
   <si>
-    <t xml:space="preserve">2020-11</t>
+    <t xml:space="preserve">2021-10</t>
   </si>
   <si>
     <t xml:space="preserve">FA</t>
@@ -485,8 +485,8 @@
   </sheetPr>
   <dimension ref="B1:AM1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="102" zoomScaleNormal="102" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="102" zoomScaleNormal="102" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -973,11 +973,11 @@
   </sheetPr>
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="16.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="12" width="17.44"/>

</xml_diff>